<commit_message>
AnnotationTransformer, cross browser support
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,21 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53DED5C-00F9-440A-A6FC-B88943534E7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5C1413-9FED-4FF3-AE62-569F68AC2C55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -92,33 +91,6 @@
   </si>
   <si>
     <t>firefox</t>
-  </si>
-  <si>
-    <t>amazonTest</t>
-  </si>
-  <si>
-    <t>To check whether the amazon test is working or not</t>
-  </si>
-  <si>
-    <t>menutext</t>
-  </si>
-  <si>
-    <t>Laptops</t>
-  </si>
-  <si>
-    <t>YWRtaW4xMjM=</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>79.0.3945.117</t>
-  </si>
-  <si>
-    <t>88.0.4324.96</t>
-  </si>
-  <si>
-    <t>69.0</t>
   </si>
 </sst>
 </file>
@@ -506,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,24 +550,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.21875" customWidth="1"/>
     <col min="2" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,48 +576,36 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -657,23 +615,17 @@
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>33</v>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -683,23 +635,17 @@
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -709,156 +655,34 @@
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>31</v>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42DCC63-8D53-4C9E-A806-695B5C2F9AD9}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new amazon test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5C1413-9FED-4FF3-AE62-569F68AC2C55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DC5D44-7844-481D-8D4F-803534E643E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>menutext</t>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+  <si>
+    <t>amazonTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To check whether amazon test is executed </t>
   </si>
 </sst>
 </file>
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -533,12 +545,29 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -550,22 +579,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.109375" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,8 +614,11 @@
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -604,8 +637,11 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,8 +660,11 @@
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -644,8 +683,11 @@
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -664,8 +706,11 @@
       <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -684,8 +729,58 @@
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
custom exception, decode password
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DC5D44-7844-481D-8D4F-803534E643E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D633D2FD-81C8-4632-B635-987BAACCCC3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>testname</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve">To check whether amazon test is executed </t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -562,7 +565,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -582,7 +585,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,13 +629,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
@@ -655,7 +658,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
@@ -669,7 +672,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -678,7 +681,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -701,7 +704,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
@@ -724,7 +727,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
@@ -738,7 +741,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>23</v>
@@ -761,7 +764,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>

</xml_diff>